<commit_message>
modulacao das janelas e melhoramento
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -2442,6 +2442,60 @@
         </is>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>kkk</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>feijão</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>feijão branco</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2453,7 +2507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
@@ -2577,6 +2631,111 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SAIDA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>22</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-12-04 17:02:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SAIDA</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-12-04 17:02:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SAIDA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-12-04 17:02:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-12-04 17:10:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>111</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2025-12-04 17:25:00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>

<commit_message>
janela de movimentos finalizados
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -2496,6 +2496,61 @@
         <v>0</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>vassoura 3</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>arroz 5L</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>5 L</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2507,7 +2562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
@@ -2736,6 +2791,90 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>11</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-12-05 16:27:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>49</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>11</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-12-09 14:44:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-12-09 15:22:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>84</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>22</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-12-09 15:22:50</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>

<commit_message>
adicionando icone as janelas e alternancia de cores nas tabelas
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -2541,13 +2541,102 @@
           <t>arroz 5L</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr">
         <is>
           <t>5 L</t>
         </is>
       </c>
       <c r="E92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>rr</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>alcool isoproponiu</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>5 L</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>alcool iso  do bom</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>PCT C/10</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>arroz soltinho</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>feijão pretola</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2562,7 +2651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
@@ -2875,6 +2964,48 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>11</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-12-16 16:39:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>11</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2025-12-16 16:39:59</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>

<commit_message>
adicionando a tabela de movimentações
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -2651,7 +2651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
@@ -3006,6 +3006,29 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Álcool</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>66</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2025-12-18 16:51:20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>

<commit_message>
adicionando janela de movimento
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -2640,6 +2640,25 @@
         <v>0</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>ee</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2651,7 +2670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
@@ -3029,6 +3048,29 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Esponja Dupla Face</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2026-01-06 15:06:26</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>

<commit_message>
janela de movimentação concluida
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -2193,25 +2193,25 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="n">
+      <c r="A99" s="8" t="n">
         <v>98</v>
       </c>
-      <c r="B99" t="inlineStr">
+      <c r="B99" s="8" t="inlineStr">
         <is>
           <t>gfff</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr">
+      <c r="C99" s="8" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr">
+      <c r="D99" s="8" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E99" t="n">
+      <c r="E99" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2228,7 +2228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
@@ -2629,6 +2629,29 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Detergente</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>12</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2026-01-18 19:47:06</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
selecionar, salvar e carregar caminho da planilha concluido
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -2630,23 +2630,23 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="8" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="8" t="inlineStr">
         <is>
           <t>Detergente</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="8" t="inlineStr">
         <is>
           <t>ENTRADA</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E19" s="8" t="inlineStr">
         <is>
           <t>2026-01-18 19:47:06</t>
         </is>

</xml_diff>

<commit_message>
correcao do modo de calcular o estoque de produtos
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,351 @@
         <is>
           <t>Estoque</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>prof</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>rd</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>rr</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>LITRO</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ddf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>dew</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>LITRO</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>faw</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>LITRO</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>gseg</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>esefse</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>LITRO</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>fse\ef</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>LITRO</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>fs\ef</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>\ef\s</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>LITRO</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>sefs</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>LITRO</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sf\es</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LITRO</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>\efse</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>LITRO</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>\fefsdf\ese\e</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>LITRO</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -460,7 +805,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,6 +845,110 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>esefse</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2026-02-26 16:46:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>rr</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2026-02-26 16:48:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>dew</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2026-02-26 17:01:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>prof</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2026-02-26 17:01:21</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>